<commit_message>
added gef sorting based on bovenkant_filter
because filternummer is random in GEF
</commit_message>
<xml_diff>
--- a/output/GTA_result.xlsx
+++ b/output/GTA_result.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:AN28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,6 +621,16 @@
       <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>gefnaam_nr</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>bovenkant filter (gef)</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Filternummer (gef)</t>
         </is>
       </c>
     </row>
@@ -671,7 +681,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>0.600000</t>
+          <t>0.630000</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr"/>
@@ -700,6 +710,12 @@
         <is>
           <t>PB_1_001_04P001442_1</t>
         </is>
+      </c>
+      <c r="AM2" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -779,6 +795,12 @@
           <t>PB_1_001_04P001442_2</t>
         </is>
       </c>
+      <c r="AM3" t="n">
+        <v>9.24</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -827,7 +849,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>0.630000</t>
+          <t>0.600000</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr"/>
@@ -856,6 +878,12 @@
         <is>
           <t>PB_1_001_04P001442_3</t>
         </is>
+      </c>
+      <c r="AM4" t="n">
+        <v>21.24</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -935,6 +963,12 @@
           <t>PB_1_002_04P001442_1</t>
         </is>
       </c>
+      <c r="AM5" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1013,6 +1047,12 @@
           <t>PB_1_002_04P001442_2</t>
         </is>
       </c>
+      <c r="AM6" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1091,6 +1131,12 @@
           <t>PB_1_002_04P001442_3</t>
         </is>
       </c>
+      <c r="AM7" t="n">
+        <v>24.25</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1169,6 +1215,12 @@
           <t>PB_1_003_04P001442_1</t>
         </is>
       </c>
+      <c r="AM8" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1247,6 +1299,12 @@
           <t>PB_1_003_04P001442_2</t>
         </is>
       </c>
+      <c r="AM9" t="n">
+        <v>8.869999999999999</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1325,6 +1383,12 @@
           <t>PB_1_003_04P001442_3</t>
         </is>
       </c>
+      <c r="AM10" t="n">
+        <v>28.870001</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1403,6 +1467,12 @@
           <t>PB_1_004_04P001442_1</t>
         </is>
       </c>
+      <c r="AM11" t="n">
+        <v>-9.720000000000001</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1481,6 +1551,12 @@
           <t>PB_1_004_04P001442_2</t>
         </is>
       </c>
+      <c r="AM12" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1559,6 +1635,12 @@
           <t>PB_1_004_04P001442_3</t>
         </is>
       </c>
+      <c r="AM13" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1637,6 +1719,12 @@
           <t>PB_1_005_04P001442_1</t>
         </is>
       </c>
+      <c r="AM14" t="n">
+        <v>-3.72</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1715,6 +1803,12 @@
           <t>PB_1_005_04P001442_2</t>
         </is>
       </c>
+      <c r="AM15" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1793,6 +1887,12 @@
           <t>PB_1_005_04P001442_3</t>
         </is>
       </c>
+      <c r="AM16" t="n">
+        <v>17.030001</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1871,6 +1971,12 @@
           <t>PB_2_001_04P001442_1</t>
         </is>
       </c>
+      <c r="AM17" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1949,6 +2055,12 @@
           <t>PB_2_001_04P001442_2</t>
         </is>
       </c>
+      <c r="AM18" t="n">
+        <v>8.390000000000001</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2027,6 +2139,12 @@
           <t>PB_2_001_04P001442_3</t>
         </is>
       </c>
+      <c r="AM19" t="n">
+        <v>28.389999</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2075,7 +2193,7 @@
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>0.600000</t>
+          <t>0.650000</t>
         </is>
       </c>
       <c r="Z20" t="inlineStr"/>
@@ -2104,6 +2222,12 @@
         <is>
           <t>PB_2_002_04P001442_1</t>
         </is>
+      </c>
+      <c r="AM20" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -2183,6 +2307,12 @@
           <t>PB_2_002_04P001442_2</t>
         </is>
       </c>
+      <c r="AM21" t="n">
+        <v>7.97</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2231,7 +2361,7 @@
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>0.650000</t>
+          <t>0.600000</t>
         </is>
       </c>
       <c r="Z22" t="inlineStr"/>
@@ -2260,6 +2390,12 @@
         <is>
           <t>PB_2_002_04P001442_3</t>
         </is>
+      </c>
+      <c r="AM22" t="n">
+        <v>23.969999</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -2339,6 +2475,12 @@
           <t>PB_2_003_04P001442_1</t>
         </is>
       </c>
+      <c r="AM23" t="n">
+        <v>-0.88</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2417,6 +2559,12 @@
           <t>PB_2_003_04P001442_2</t>
         </is>
       </c>
+      <c r="AM24" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2495,6 +2643,12 @@
           <t>PB_2_003_04P001442_3</t>
         </is>
       </c>
+      <c r="AM25" t="n">
+        <v>21.120001</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2573,6 +2727,12 @@
           <t>PB_6_001_04P001442_1</t>
         </is>
       </c>
+      <c r="AM26" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2651,6 +2811,12 @@
           <t>PB_6_001_04P001442_2</t>
         </is>
       </c>
+      <c r="AM27" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2729,6 +2895,12 @@
           <t>PB_6_001_04P001442_3</t>
         </is>
       </c>
+      <c r="AM28" t="n">
+        <v>21</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>